<commit_message>
Removed zeros from cps in calibration
</commit_message>
<xml_diff>
--- a/data_processing/2024/OES/data/spectra_scaling_dalpha.xlsx
+++ b/data_processing/2024/OES/data/spectra_scaling_dalpha.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
         <v>433.98749</v>
       </c>
       <c r="E2" t="n">
-        <v>32479288815271.73</v>
+        <v>33302736195339.95</v>
       </c>
       <c r="F2" t="n">
         <v>-0.05748999999997295</v>
@@ -507,7 +507,7 @@
         <v>433.98749</v>
       </c>
       <c r="E3" t="n">
-        <v>25165786406125.34</v>
+        <v>25803814566204.28</v>
       </c>
       <c r="F3" t="n">
         <v>-0.05748999999997295</v>
@@ -531,7 +531,7 @@
         <v>433.98749</v>
       </c>
       <c r="E4" t="n">
-        <v>25123154907153.24</v>
+        <v>25760102230877.15</v>
       </c>
       <c r="F4" t="n">
         <v>-0.05748999999997295</v>
@@ -555,7 +555,7 @@
         <v>433.98749</v>
       </c>
       <c r="E5" t="n">
-        <v>26184816752523.01</v>
+        <v>26848680388055.98</v>
       </c>
       <c r="F5" t="n">
         <v>-0.05748999999997295</v>
@@ -579,7 +579,7 @@
         <v>433.98749</v>
       </c>
       <c r="E6" t="n">
-        <v>17871949494891.89</v>
+        <v>18325057014332.43</v>
       </c>
       <c r="F6" t="n">
         <v>-0.05748999999997295</v>
@@ -603,7 +603,7 @@
         <v>433.98749</v>
       </c>
       <c r="E7" t="n">
-        <v>19089560113920.9</v>
+        <v>19573537714288.55</v>
       </c>
       <c r="F7" t="n">
         <v>-0.05748999999997295</v>
@@ -627,7 +627,7 @@
         <v>433.98749</v>
       </c>
       <c r="E8" t="n">
-        <v>21353430230303.98</v>
+        <v>21894803727692.43</v>
       </c>
       <c r="F8" t="n">
         <v>-0.05748999999997295</v>
@@ -651,7 +651,7 @@
         <v>433.66614</v>
       </c>
       <c r="E9" t="n">
-        <v>109048567431.1062</v>
+        <v>121353577272.7677</v>
       </c>
       <c r="F9" t="n">
         <v>0.2638600000000224</v>
@@ -675,7 +675,7 @@
         <v>433.98749</v>
       </c>
       <c r="E10" t="n">
-        <v>79097685805412.98</v>
+        <v>81443109428571.41</v>
       </c>
       <c r="F10" t="n">
         <v>-0.05748999999997295</v>
@@ -699,7 +699,7 @@
         <v>433.98749</v>
       </c>
       <c r="E11" t="n">
-        <v>54921394156509.16</v>
+        <v>56549936558980.52</v>
       </c>
       <c r="F11" t="n">
         <v>-0.05748999999997295</v>
@@ -723,7 +723,7 @@
         <v>433.98749</v>
       </c>
       <c r="E12" t="n">
-        <v>45956497324942.22</v>
+        <v>47319210448164.34</v>
       </c>
       <c r="F12" t="n">
         <v>-0.05748999999997295</v>
@@ -747,7 +747,7 @@
         <v>433.98749</v>
       </c>
       <c r="E13" t="n">
-        <v>37661854544599.03</v>
+        <v>38778612923070</v>
       </c>
       <c r="F13" t="n">
         <v>-0.05748999999997295</v>
@@ -771,7 +771,7 @@
         <v>433.98749</v>
       </c>
       <c r="E14" t="n">
-        <v>26701482618698.79</v>
+        <v>27493241409990.3</v>
       </c>
       <c r="F14" t="n">
         <v>-0.05748999999997295</v>
@@ -795,7 +795,7 @@
         <v>433.98749</v>
       </c>
       <c r="E15" t="n">
-        <v>27115903235708.43</v>
+        <v>27919950526911.94</v>
       </c>
       <c r="F15" t="n">
         <v>-0.05748999999997295</v>
@@ -819,7 +819,7 @@
         <v>433.98749</v>
       </c>
       <c r="E16" t="n">
-        <v>20456205028422.19</v>
+        <v>21062777344986.1</v>
       </c>
       <c r="F16" t="n">
         <v>-0.05748999999997295</v>
@@ -843,7 +843,7 @@
         <v>433.98749</v>
       </c>
       <c r="E17" t="n">
-        <v>21652385305943.98</v>
+        <v>22294427048090.8</v>
       </c>
       <c r="F17" t="n">
         <v>-0.05748999999997295</v>
@@ -867,7 +867,7 @@
         <v>433.98749</v>
       </c>
       <c r="E18" t="n">
-        <v>22811568330614.32</v>
+        <v>23487982446895</v>
       </c>
       <c r="F18" t="n">
         <v>-0.05748999999997295</v>
@@ -891,7 +891,7 @@
         <v>433.93719</v>
       </c>
       <c r="E19" t="n">
-        <v>64289000114769.82</v>
+        <v>66840695350615.36</v>
       </c>
       <c r="F19" t="n">
         <v>-0.007189999999980046</v>
@@ -915,7 +915,7 @@
         <v>433.93719</v>
       </c>
       <c r="E20" t="n">
-        <v>51769484163159.66</v>
+        <v>53824267187712.68</v>
       </c>
       <c r="F20" t="n">
         <v>-0.007189999999980046</v>
@@ -939,7 +939,7 @@
         <v>433.93719</v>
       </c>
       <c r="E21" t="n">
-        <v>42589604348231.76</v>
+        <v>44280028687044.3</v>
       </c>
       <c r="F21" t="n">
         <v>-0.007189999999980046</v>
@@ -963,7 +963,7 @@
         <v>433.93719</v>
       </c>
       <c r="E22" t="n">
-        <v>35442404424676</v>
+        <v>36849149192146.41</v>
       </c>
       <c r="F22" t="n">
         <v>-0.007189999999980046</v>
@@ -987,7 +987,7 @@
         <v>433.93719</v>
       </c>
       <c r="E23" t="n">
-        <v>31401012996539.87</v>
+        <v>32647350863374.83</v>
       </c>
       <c r="F23" t="n">
         <v>-0.007189999999980046</v>
@@ -1011,7 +1011,7 @@
         <v>433.93719</v>
       </c>
       <c r="E24" t="n">
-        <v>31563207941644</v>
+        <v>32815983489388</v>
       </c>
       <c r="F24" t="n">
         <v>-0.007189999999980046</v>
@@ -1035,7 +1035,7 @@
         <v>433.91003</v>
       </c>
       <c r="E25" t="n">
-        <v>31915850992491.72</v>
+        <v>33418363146838.54</v>
       </c>
       <c r="F25" t="n">
         <v>0.01997000000000071</v>
@@ -1059,7 +1059,7 @@
         <v>433.93719</v>
       </c>
       <c r="E26" t="n">
-        <v>31615230165850.36</v>
+        <v>32870070528126.05</v>
       </c>
       <c r="F26" t="n">
         <v>-0.007189999999980046</v>
@@ -1083,7 +1083,7 @@
         <v>433.93719</v>
       </c>
       <c r="E27" t="n">
-        <v>29970946566196.91</v>
+        <v>31160523654504.68</v>
       </c>
       <c r="F27" t="n">
         <v>-0.007189999999980046</v>
@@ -1107,7 +1107,7 @@
         <v>433.93719</v>
       </c>
       <c r="E28" t="n">
-        <v>33293287356088.04</v>
+        <v>34614731500195.18</v>
       </c>
       <c r="F28" t="n">
         <v>-0.007189999999980046</v>
@@ -1131,7 +1131,7 @@
         <v>433.93719</v>
       </c>
       <c r="E29" t="n">
-        <v>32803706476449.63</v>
+        <v>34105718661809.49</v>
       </c>
       <c r="F29" t="n">
         <v>-0.007189999999980046</v>
@@ -1155,7 +1155,7 @@
         <v>433.91003</v>
       </c>
       <c r="E30" t="n">
-        <v>72246286959625.72</v>
+        <v>75647447226002.52</v>
       </c>
       <c r="F30" t="n">
         <v>0.01997000000000071</v>
@@ -1179,7 +1179,7 @@
         <v>433.91003</v>
       </c>
       <c r="E31" t="n">
-        <v>70656663128276.61</v>
+        <v>73982988193549</v>
       </c>
       <c r="F31" t="n">
         <v>0.01997000000000071</v>
@@ -1203,7 +1203,7 @@
         <v>433.88287</v>
       </c>
       <c r="E32" t="n">
-        <v>114027810597489.8</v>
+        <v>120243122971215.3</v>
       </c>
       <c r="F32" t="n">
         <v>0.04712999999998146</v>
@@ -1227,7 +1227,7 @@
         <v>433.88287</v>
       </c>
       <c r="E33" t="n">
-        <v>75307482558746.62</v>
+        <v>79412266520912.78</v>
       </c>
       <c r="F33" t="n">
         <v>0.04712999999998146</v>
@@ -1251,7 +1251,7 @@
         <v>433.88287</v>
       </c>
       <c r="E34" t="n">
-        <v>49433531910863.45</v>
+        <v>52128004785091.45</v>
       </c>
       <c r="F34" t="n">
         <v>0.04712999999998146</v>
@@ -1275,7 +1275,7 @@
         <v>433.88287</v>
       </c>
       <c r="E35" t="n">
-        <v>42437384297400.83</v>
+        <v>44750518245602.66</v>
       </c>
       <c r="F35" t="n">
         <v>0.04712999999998146</v>
@@ -1299,7 +1299,7 @@
         <v>433.88287</v>
       </c>
       <c r="E36" t="n">
-        <v>36526599250911.48</v>
+        <v>38517554116261.69</v>
       </c>
       <c r="F36" t="n">
         <v>0.04712999999998146</v>
@@ -1323,7 +1323,7 @@
         <v>433.88287</v>
       </c>
       <c r="E37" t="n">
-        <v>29560997809773.55</v>
+        <v>31172278728911.03</v>
       </c>
       <c r="F37" t="n">
         <v>0.04712999999998146</v>
@@ -1347,7 +1347,7 @@
         <v>433.91003</v>
       </c>
       <c r="E38" t="n">
-        <v>27582051199888.14</v>
+        <v>28880539752782.98</v>
       </c>
       <c r="F38" t="n">
         <v>0.01997000000000071</v>
@@ -1371,7 +1371,7 @@
         <v>433.91003</v>
       </c>
       <c r="E39" t="n">
-        <v>26954860043961.8</v>
+        <v>28223822129425.15</v>
       </c>
       <c r="F39" t="n">
         <v>0.01997000000000071</v>
@@ -1395,7 +1395,7 @@
         <v>433.91003</v>
       </c>
       <c r="E40" t="n">
-        <v>23298319370455.12</v>
+        <v>24395141386518.48</v>
       </c>
       <c r="F40" t="n">
         <v>0.01997000000000071</v>
@@ -1419,9 +1419,33 @@
         <v>433.91003</v>
       </c>
       <c r="E41" t="n">
-        <v>21779044849089.14</v>
+        <v>22804343519756.54</v>
       </c>
       <c r="F41" t="n">
+        <v>0.01997000000000071</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>echelle_20241003</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>MechelleSpect_001.csv</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>433.93</v>
+      </c>
+      <c r="D42" t="n">
+        <v>433.91003</v>
+      </c>
+      <c r="E42" t="n">
+        <v>93517799954142.44</v>
+      </c>
+      <c r="F42" t="n">
         <v>0.01997000000000071</v>
       </c>
     </row>

</xml_diff>